<commit_message>
feita a analise dos dados
</commit_message>
<xml_diff>
--- a/exercicios_extras/faltas_tratadas.xlsx
+++ b/exercicios_extras/faltas_tratadas.xlsx
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="H2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -600,7 +600,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -636,7 +636,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -672,7 +672,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -748,7 +748,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -764,7 +764,7 @@
         </is>
       </c>
       <c r="H9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -816,7 +816,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -888,7 +888,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -924,7 +924,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -996,7 +996,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1248,7 +1248,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1448,7 +1448,7 @@
         </is>
       </c>
       <c r="H28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1752,7 +1752,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1824,7 +1824,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1968,7 +1968,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -2008,7 +2008,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2024,7 +2024,7 @@
         </is>
       </c>
       <c r="H44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -2040,7 +2040,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2112,7 +2112,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -2184,7 +2184,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2220,7 +2220,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -2328,7 +2328,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -2652,7 +2652,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -2692,7 +2692,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2708,7 +2708,7 @@
         </is>
       </c>
       <c r="H63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -2760,7 +2760,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2832,7 +2832,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -3228,7 +3228,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D78" t="n">
@@ -3516,7 +3516,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -3912,7 +3912,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D97" t="n">
@@ -3948,11 +3948,11 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -3968,7 +3968,7 @@
         </is>
       </c>
       <c r="H98" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -3984,7 +3984,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -4128,7 +4128,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -4164,7 +4164,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D104" t="n">
@@ -4236,7 +4236,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D106" t="n">
@@ -4416,7 +4416,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D111" t="n">
@@ -4596,7 +4596,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D116" t="n">
@@ -4812,7 +4812,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -4884,7 +4884,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D124" t="n">
@@ -4956,7 +4956,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -5244,7 +5244,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -5532,7 +5532,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -5676,7 +5676,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D146" t="n">
@@ -5784,7 +5784,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -5964,7 +5964,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -6036,7 +6036,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -6252,7 +6252,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D162" t="n">
@@ -6288,7 +6288,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -6324,7 +6324,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -6504,7 +6504,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D169" t="n">
@@ -6792,7 +6792,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -6900,7 +6900,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -7260,7 +7260,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -7404,7 +7404,7 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D194" t="n">
@@ -7476,11 +7476,11 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -7496,7 +7496,7 @@
         </is>
       </c>
       <c r="H196" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197">
@@ -7584,7 +7584,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -7620,7 +7620,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -7660,7 +7660,7 @@
         </is>
       </c>
       <c r="D201" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -7676,7 +7676,7 @@
         </is>
       </c>
       <c r="H201" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202">
@@ -7692,7 +7692,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -7872,7 +7872,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -7908,7 +7908,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D208" t="n">
@@ -8124,7 +8124,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -8232,7 +8232,7 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>Manha</t>
+          <t>Manhã</t>
         </is>
       </c>
       <c r="D217" t="n">

</xml_diff>